<commit_message>
Modification suivi des charges et ajout documentation serveur Apache
Modification suivi des charges et ajout documentation serveur Apache
</commit_message>
<xml_diff>
--- a/documents/PMP/Suivi_du_projet/Suivi_METAHRI_Elie.xlsx
+++ b/documents/PMP/Suivi_du_projet/Suivi_METAHRI_Elie.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>TACHES</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>Heures</t>
+  </si>
+  <si>
+    <t>Mise en place serveur Apache</t>
+  </si>
+  <si>
+    <t>Rédaction documentation serveur Apache</t>
   </si>
 </sst>
 </file>
@@ -492,7 +498,7 @@
   <dimension ref="B2:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,8 +536,8 @@
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="6">
-        <f>SUM(D3:D19)</f>
-        <v>66.2</v>
+        <f>SUM(D3:D21)</f>
+        <v>68.7</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>17</v>
@@ -712,14 +718,26 @@
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="3">
+        <v>42325</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="3">
+        <v>42325</v>
+      </c>
+      <c r="D21" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>

</xml_diff>